<commit_message>
Update. 20+ additional surveys included
</commit_message>
<xml_diff>
--- a/Check means on HIST data.xlsx
+++ b/Check means on HIST data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\02.personal\wb463998\Historical data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2DE7923-C450-44AD-9590-F90BDF142720}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EE9667-A6CC-484D-AD76-FAF11EE19FCE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="raw" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw!$A$1:$J$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">raw!$A$1:$J$104</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="59">
   <si>
     <t>countrycode</t>
   </si>
@@ -196,6 +196,18 @@
   </si>
   <si>
     <t>Fixed do &amp; dta</t>
+  </si>
+  <si>
+    <t>CHL</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>VEN</t>
+  </si>
+  <si>
+    <t>LKA</t>
   </si>
 </sst>
 </file>
@@ -274,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -311,6 +323,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,10 +641,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J82"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56:J56"/>
+      <selection activeCell="L104" sqref="L104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,7 +654,7 @@
     <col min="2" max="2" width="8.7265625" style="4"/>
     <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.90625" style="4" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="8.90625" style="4" customWidth="1"/>
     <col min="6" max="6" width="5.453125" customWidth="1"/>
     <col min="7" max="8" width="9.90625" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
@@ -673,7 +690,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -704,7 +721,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -734,7 +751,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -764,7 +781,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -795,7 +812,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -826,7 +843,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -857,7 +874,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -887,7 +904,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -917,7 +934,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -947,7 +964,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -977,7 +994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1007,7 +1024,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1054,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -1245,7 +1262,7 @@
         <v>398.3723</v>
       </c>
       <c r="I20" s="9">
-        <f t="shared" ref="I20:I72" si="1">D20/H20</f>
+        <f t="shared" ref="I20:I83" si="1">D20/H20</f>
         <v>999.99995716577189</v>
       </c>
     </row>
@@ -1303,7 +1320,7 @@
         <v>1000.0000688139837</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -1333,7 +1350,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1363,1352 +1380,1360 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1987</v>
+      </c>
+      <c r="C25">
+        <v>0.56210157999999999</v>
+      </c>
+      <c r="D25">
+        <v>299.16523000000001</v>
+      </c>
+      <c r="E25">
+        <v>11.674734000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.56210159999999998</v>
+      </c>
+      <c r="H25">
+        <v>299.16520000000003</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0000001002790431</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26">
+        <v>1992</v>
+      </c>
+      <c r="C26">
+        <v>0.51453673</v>
+      </c>
+      <c r="D26">
+        <v>292.72201000000001</v>
+      </c>
+      <c r="E26">
+        <v>8.8905398000000009</v>
+      </c>
+      <c r="G26">
+        <v>0.51453669999999996</v>
+      </c>
+      <c r="H26">
+        <v>292.72199999999998</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" si="1"/>
+        <v>1.000000034162106</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27">
+        <v>1996</v>
+      </c>
+      <c r="C27">
+        <v>0.56936907999999997</v>
+      </c>
+      <c r="D27">
+        <v>265.64663000000002</v>
+      </c>
+      <c r="E27">
+        <v>16.558036999999999</v>
+      </c>
+      <c r="G27">
+        <v>0.56933040000000001</v>
+      </c>
+      <c r="H27">
+        <v>265.67700000000002</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.99988568826055702</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28">
+        <v>1999</v>
+      </c>
+      <c r="C28">
+        <v>0.58739600000000003</v>
+      </c>
+      <c r="D28">
+        <v>254.07632000000001</v>
+      </c>
+      <c r="E28">
+        <v>20.072175000000001</v>
+      </c>
+      <c r="G28">
+        <v>0.58739560000000002</v>
+      </c>
+      <c r="H28">
+        <v>254.0771</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="shared" si="1"/>
+        <v>0.99999693006571633</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29">
+        <v>2000</v>
+      </c>
+      <c r="C29">
+        <v>0.58682893000000003</v>
+      </c>
+      <c r="D29">
+        <v>283.39211</v>
+      </c>
+      <c r="E29">
+        <v>16.369323000000001</v>
+      </c>
+      <c r="G29">
+        <v>0.58682889999999999</v>
+      </c>
+      <c r="H29">
+        <v>283.39210000000003</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0000000352867986</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B30" s="5">
         <v>2002</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C30" s="3">
         <v>0.39997838987954998</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D30" s="1">
         <v>1610.069167136</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E30" s="6">
         <v>1.204879321614E-2</v>
       </c>
-      <c r="G25" s="8">
+      <c r="G30" s="8">
         <v>0.39997840000000001</v>
       </c>
-      <c r="H25">
+      <c r="H30">
         <v>134.1671</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I30" s="9">
         <f t="shared" si="1"/>
         <v>12.000476772144587</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="J30" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B31" s="5">
         <v>2000</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C31" s="3">
         <v>0.63261969178318</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D31" s="1">
         <v>1873.2307541591999</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E31" s="6">
         <v>3.4963564285638999</v>
       </c>
-      <c r="G26" s="8">
+      <c r="G31" s="8">
         <v>0.63261970000000001</v>
       </c>
-      <c r="H26">
+      <c r="H31">
         <v>156.09630000000001</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I31" s="9">
         <f t="shared" si="1"/>
         <v>12.000481460221669</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="J31" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B32" s="5">
         <v>1993</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C32" s="3">
         <v>0.43610226254146001</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D32" s="1">
         <f>75085.636529988/12</f>
         <v>6257.1363774989995</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E32" s="6">
         <v>0</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G32" s="8">
         <v>0.4361023</v>
       </c>
-      <c r="H27">
+      <c r="H32">
         <v>62.571359999999999</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I32" s="9">
         <f t="shared" si="1"/>
         <v>100.00000603309564</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B33" s="5">
         <v>2001</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C33" s="3">
         <v>0.59476618320963004</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D33" s="1">
         <v>975.65799114943002</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E33" s="6">
         <v>4.5070635513359001</v>
       </c>
-      <c r="G28" s="8">
+      <c r="G33" s="8">
         <v>0.59476620000000002</v>
       </c>
-      <c r="H28">
+      <c r="H33">
         <v>81.301580000000001</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I33" s="9">
         <f t="shared" si="1"/>
         <v>12.000480078608927</v>
       </c>
-      <c r="J28" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="J33" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B34" s="4">
         <v>1993</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C34" s="8">
         <v>0.35353240000000002</v>
       </c>
-      <c r="D29" s="10">
-        <v>1229.9129</v>
-      </c>
-      <c r="E29" s="11">
+      <c r="D34" s="10">
+        <v>86.172799999999995</v>
+      </c>
+      <c r="E34" s="11">
+        <v>40.091000000000001</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G34" s="8">
+        <v>0.35354029999999997</v>
+      </c>
+      <c r="H34">
+        <v>86.18</v>
+      </c>
+      <c r="I34" s="9">
+        <f>D34/H34</f>
+        <v>0.99991645393362716</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1996</v>
+      </c>
+      <c r="C35" s="8">
+        <v>0.37549613999999998</v>
+      </c>
+      <c r="D35" s="10">
+        <v>1234.0694000000001</v>
+      </c>
+      <c r="E35" s="11">
+        <v>2.17016E-3</v>
+      </c>
+      <c r="F35" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0.37549929999999998</v>
+      </c>
+      <c r="H35">
+        <v>102.8404</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" si="1"/>
+        <v>11.999850253402361</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1998</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.33776075999999999</v>
+      </c>
+      <c r="D36" s="10">
+        <v>857.09517000000005</v>
+      </c>
+      <c r="E36" s="11">
+        <v>0.27223646000000001</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0.3377444</v>
+      </c>
+      <c r="H36">
+        <v>71.421279999999996</v>
+      </c>
+      <c r="I36" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000557396899078</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1999</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.35375032000000001</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1150.6957</v>
+      </c>
+      <c r="E37" s="11">
         <v>0</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F37" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="8">
-        <v>0.35354029999999997</v>
-      </c>
-      <c r="H29">
-        <v>86.18</v>
-      </c>
-      <c r="I29" s="9">
-        <f t="shared" si="1"/>
-        <v>14.271442330006961</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="4">
+      <c r="G37" s="8">
+        <v>0.35373270000000001</v>
+      </c>
+      <c r="H37">
+        <v>95.889139999999998</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000271355025189</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1990</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.41114000000000001</v>
+      </c>
+      <c r="D38" s="10">
+        <v>231.98740000000001</v>
+      </c>
+      <c r="E38" s="11">
+        <v>4.57</v>
+      </c>
+      <c r="F38" s="14"/>
+      <c r="G38">
+        <v>0.41114079999999997</v>
+      </c>
+      <c r="H38">
+        <v>231.9905</v>
+      </c>
+      <c r="I38" s="9">
+        <f t="shared" si="1"/>
+        <v>0.9999866373838584</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="5">
         <v>1996</v>
       </c>
-      <c r="C30" s="8">
-        <v>0.37549613999999998</v>
-      </c>
-      <c r="D30" s="10">
-        <v>1234.0694000000001</v>
-      </c>
-      <c r="E30" s="11">
-        <v>2.17016E-3</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G30" s="8">
-        <v>0.37549929999999998</v>
-      </c>
-      <c r="H30">
-        <v>102.8404</v>
-      </c>
-      <c r="I30" s="9">
-        <f t="shared" si="1"/>
-        <v>11.999850253402361</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="4">
-        <v>1998</v>
-      </c>
-      <c r="C31" s="8">
-        <v>0.33776075999999999</v>
-      </c>
-      <c r="D31" s="10">
-        <v>857.09517000000005</v>
-      </c>
-      <c r="E31" s="11">
-        <v>0.27223646000000001</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G31" s="8">
-        <v>0.3377444</v>
-      </c>
-      <c r="H31">
-        <v>71.421279999999996</v>
-      </c>
-      <c r="I31" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000557396899078</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="4">
+      <c r="C39" s="3">
+        <v>0.40394902306302</v>
+      </c>
+      <c r="D39" s="1">
+        <v>3009.5164703894998</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+      <c r="G39" s="8">
+        <v>0.403949</v>
+      </c>
+      <c r="H39">
+        <v>250.78299999999999</v>
+      </c>
+      <c r="I39" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000480377017182</v>
+      </c>
+      <c r="J39" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="5">
         <v>1999</v>
       </c>
-      <c r="C32" s="8">
-        <v>0.35375032000000001</v>
-      </c>
-      <c r="D32" s="10">
-        <v>1150.6957</v>
-      </c>
-      <c r="E32" s="11">
-        <v>0</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="G32" s="8">
-        <v>0.35373270000000001</v>
-      </c>
-      <c r="H32">
-        <v>95.889139999999998</v>
-      </c>
-      <c r="I32" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000271355025189</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+      <c r="C40" s="3">
+        <v>0.44080198676408</v>
+      </c>
+      <c r="D40" s="1">
+        <v>4044.1052947211001</v>
+      </c>
+      <c r="E40" s="6">
+        <v>5.5605042024839998E-2</v>
+      </c>
+      <c r="G40" s="8">
+        <v>0.44080200000000003</v>
+      </c>
+      <c r="H40">
+        <v>336.99529999999999</v>
+      </c>
+      <c r="I40" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000479812985819</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="5">
-        <v>1996</v>
-      </c>
-      <c r="C33" s="3">
-        <v>0.40394902306302</v>
-      </c>
-      <c r="D33" s="1">
-        <v>3009.5164703894998</v>
-      </c>
-      <c r="E33" s="6">
-        <v>0</v>
-      </c>
-      <c r="G33" s="8">
-        <v>0.403949</v>
-      </c>
-      <c r="H33">
-        <v>250.78299999999999</v>
-      </c>
-      <c r="I33" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000480377017182</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
+      <c r="B41" s="5">
+        <v>2002</v>
+      </c>
+      <c r="C41" s="3">
+        <v>0.48315962507707999</v>
+      </c>
+      <c r="D41" s="1">
+        <v>4402.6711349060997</v>
+      </c>
+      <c r="E41" s="6">
+        <v>9.1638376652899995E-3</v>
+      </c>
+      <c r="G41" s="8">
+        <v>0.48315960000000002</v>
+      </c>
+      <c r="H41">
+        <v>366.87459999999999</v>
+      </c>
+      <c r="I41" s="9">
+        <f t="shared" si="1"/>
+        <v>12.00047955052244</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="5">
-        <v>1999</v>
-      </c>
-      <c r="C34" s="3">
-        <v>0.44080198676408</v>
-      </c>
-      <c r="D34" s="1">
-        <v>4044.1052947211001</v>
-      </c>
-      <c r="E34" s="6">
-        <v>5.5605042024839998E-2</v>
-      </c>
-      <c r="G34" s="8">
-        <v>0.44080200000000003</v>
-      </c>
-      <c r="H34">
-        <v>336.99529999999999</v>
-      </c>
-      <c r="I34" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000479812985819</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B35" s="5">
-        <v>2002</v>
-      </c>
-      <c r="C35" s="3">
-        <v>0.48315962507707999</v>
-      </c>
-      <c r="D35" s="1">
-        <v>4402.6711349060997</v>
-      </c>
-      <c r="E35" s="6">
-        <v>9.1638376652899995E-3</v>
-      </c>
-      <c r="G35" s="8">
-        <v>0.48315960000000002</v>
-      </c>
-      <c r="H35">
-        <v>366.87459999999999</v>
-      </c>
-      <c r="I35" s="9">
-        <f t="shared" si="1"/>
-        <v>12.00047955052244</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B36" s="5">
+      <c r="B42" s="5">
         <v>2004</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C42" s="3">
         <v>0.45457474397075998</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D42" s="1">
         <v>4396.1987214295996</v>
-      </c>
-      <c r="E36" s="6">
-        <v>0</v>
-      </c>
-      <c r="G36" s="8">
-        <v>0.4545747</v>
-      </c>
-      <c r="H36">
-        <v>366.33519999999999</v>
-      </c>
-      <c r="I36" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000481311731987</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A37" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="5">
-        <v>2002</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0.36954616324049</v>
-      </c>
-      <c r="D37" s="1">
-        <v>3231.5283134480001</v>
-      </c>
-      <c r="E37" s="6">
-        <v>0</v>
-      </c>
-      <c r="G37" s="8">
-        <v>0.3695465</v>
-      </c>
-      <c r="H37">
-        <v>269.2946</v>
-      </c>
-      <c r="I37" s="9">
-        <f t="shared" si="1"/>
-        <v>11.999974427441174</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="5">
-        <v>1996</v>
-      </c>
-      <c r="C38" s="3">
-        <v>0.35378308139165998</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2254.3768150501</v>
-      </c>
-      <c r="E38" s="6">
-        <v>0</v>
-      </c>
-      <c r="G38" s="8">
-        <v>0.35378310000000002</v>
-      </c>
-      <c r="H38">
-        <v>187.85720000000001</v>
-      </c>
-      <c r="I38" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000481296698236</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="5">
-        <v>1998</v>
-      </c>
-      <c r="C39" s="3">
-        <v>0.46402012792726</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1550.5460830401</v>
-      </c>
-      <c r="E39" s="6">
-        <v>0.30933749427114998</v>
-      </c>
-      <c r="G39" s="8">
-        <v>0.46402009999999999</v>
-      </c>
-      <c r="H39">
-        <v>129.20699999999999</v>
-      </c>
-      <c r="I39" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000480492853329</v>
-      </c>
-      <c r="J39" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="5">
-        <v>1997</v>
-      </c>
-      <c r="C40" s="3">
-        <v>0.34895439994757999</v>
-      </c>
-      <c r="D40" s="1">
-        <v>5791.3158023891001</v>
-      </c>
-      <c r="E40" s="6">
-        <v>0</v>
-      </c>
-      <c r="G40" s="8">
-        <v>0.34895209999999999</v>
-      </c>
-      <c r="H40">
-        <v>72.39846</v>
-      </c>
-      <c r="I40" s="9">
-        <f t="shared" si="1"/>
-        <v>79.992251249392595</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B41" s="5">
-        <v>1994</v>
-      </c>
-      <c r="C41" s="3">
-        <v>0.63240365126325004</v>
-      </c>
-      <c r="D41" s="1">
-        <v>1579.0311005271001</v>
-      </c>
-      <c r="E41" s="6">
-        <v>3.0019801980198002</v>
-      </c>
-      <c r="G41" s="8">
-        <v>0.63240410000000002</v>
-      </c>
-      <c r="H41">
-        <v>131.58510000000001</v>
-      </c>
-      <c r="I41" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000075240487714</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A42" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B42" s="5">
-        <v>1997</v>
-      </c>
-      <c r="C42" s="3">
-        <v>0.34392591743202999</v>
-      </c>
-      <c r="D42" s="1">
-        <v>3324.0256404453999</v>
       </c>
       <c r="E42" s="6">
         <v>0</v>
       </c>
       <c r="G42" s="8">
-        <v>0.34392590000000001</v>
+        <v>0.4545747</v>
       </c>
       <c r="H42">
-        <v>277.00209999999998</v>
+        <v>366.33519999999999</v>
       </c>
       <c r="I42" s="9">
         <f t="shared" si="1"/>
-        <v>12.000001590043542</v>
+        <v>12.000481311731987</v>
       </c>
       <c r="J42" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B43" s="5">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="C43" s="3">
-        <v>0.33264852906081999</v>
+        <v>0.36954616324049</v>
       </c>
       <c r="D43" s="1">
-        <v>3389.7841033217001</v>
+        <v>3231.5283134480001</v>
       </c>
       <c r="E43" s="6">
         <v>0</v>
       </c>
       <c r="G43" s="8">
-        <v>0.33264850000000001</v>
+        <v>0.3695465</v>
       </c>
       <c r="H43">
-        <v>282.47070000000002</v>
+        <v>269.2946</v>
       </c>
       <c r="I43" s="9">
         <f t="shared" si="1"/>
-        <v>12.000480415567703</v>
+        <v>11.999974427441174</v>
       </c>
       <c r="J43" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B44" s="5">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="C44" s="3">
-        <v>0.36942146402816001</v>
+        <v>0.35378308139165998</v>
       </c>
       <c r="D44" s="1">
-        <v>1651.5335344744999</v>
+        <v>2254.3768150501</v>
       </c>
       <c r="E44" s="6">
         <v>0</v>
       </c>
       <c r="G44" s="8">
-        <v>0.36942150000000001</v>
+        <v>0.35378310000000002</v>
       </c>
       <c r="H44">
-        <v>137.6223</v>
+        <v>187.85720000000001</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="1"/>
-        <v>12.000479097315624</v>
+        <v>12.000481296698236</v>
       </c>
       <c r="J44" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B45" s="5">
-        <v>1984</v>
+        <v>1998</v>
       </c>
       <c r="C45" s="3">
-        <v>0.48947361158580999</v>
+        <v>0.46402012792726</v>
       </c>
       <c r="D45" s="1">
-        <v>298.99035500367</v>
+        <v>1550.5460830401</v>
       </c>
       <c r="E45" s="6">
-        <v>8.1377779613252006</v>
+        <v>0.30933749427114998</v>
       </c>
       <c r="G45" s="8">
-        <v>0.48947459999999998</v>
+        <v>0.46402009999999999</v>
       </c>
       <c r="H45">
-        <v>298.99160000000001</v>
+        <v>129.20699999999999</v>
       </c>
       <c r="I45" s="9">
         <f t="shared" si="1"/>
-        <v>0.99999583601569408</v>
+        <v>12.000480492853329</v>
       </c>
       <c r="J45" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1992</v>
+      </c>
+      <c r="C46">
+        <v>0.34309774999999998</v>
+      </c>
+      <c r="D46" s="19">
+        <v>95.039034999999998</v>
+      </c>
+      <c r="E46" s="19">
+        <v>32.395508</v>
+      </c>
+      <c r="G46" s="8">
+        <v>0.34309859999999998</v>
+      </c>
+      <c r="H46">
+        <v>95.039119999999997</v>
+      </c>
+      <c r="I46" s="9">
+        <f t="shared" si="1"/>
+        <v>0.99999910563144945</v>
+      </c>
+      <c r="J46" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A46" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B46" s="5">
-        <v>1989</v>
-      </c>
-      <c r="C46" s="3">
-        <v>0.54342483967208999</v>
-      </c>
-      <c r="D46" s="1">
-        <v>367.25653775262998</v>
-      </c>
-      <c r="E46" s="6">
-        <v>7.0811973975678004</v>
-      </c>
-      <c r="G46" s="8">
-        <v>0.54342599999999996</v>
-      </c>
-      <c r="H46">
-        <v>367.25450000000001</v>
-      </c>
-      <c r="I46" s="9">
-        <f t="shared" si="1"/>
-        <v>1.0000055486117392</v>
-      </c>
-      <c r="J46" s="4" t="s">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B47" s="5">
+        <v>1997</v>
+      </c>
+      <c r="C47" s="3">
+        <v>0.34895439994757999</v>
+      </c>
+      <c r="D47" s="1">
+        <v>72.398690000000002</v>
+      </c>
+      <c r="E47" s="6">
+        <v>52.447000000000003</v>
+      </c>
+      <c r="G47" s="8">
+        <v>0.34895209999999999</v>
+      </c>
+      <c r="H47">
+        <v>72.39846</v>
+      </c>
+      <c r="I47" s="9">
+        <f>D47/H47</f>
+        <v>1.0000031768631543</v>
+      </c>
+      <c r="J47" s="18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B47" s="5">
-        <v>1994</v>
-      </c>
-      <c r="C47" s="3">
-        <v>0.50441236709199</v>
-      </c>
-      <c r="D47" s="1">
-        <v>449.08490898819002</v>
-      </c>
-      <c r="E47" s="6">
-        <v>1.6730619539156999</v>
-      </c>
-      <c r="G47" s="8">
-        <v>0.50441239999999998</v>
-      </c>
-      <c r="H47">
-        <v>37.422249999999998</v>
-      </c>
-      <c r="I47" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000478565243673</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B48" s="5">
-        <v>2002</v>
+        <v>1990</v>
       </c>
       <c r="C48" s="3">
-        <v>0.32892948140056999</v>
+        <v>0.32446999999999998</v>
       </c>
       <c r="D48" s="1">
-        <v>1818.2521166762001</v>
-      </c>
-      <c r="E48" s="6">
-        <v>0</v>
-      </c>
+        <v>132.55869999999999</v>
+      </c>
+      <c r="E48" s="6"/>
       <c r="G48" s="8">
-        <v>0.32892949999999999</v>
+        <v>0.32447579999999998</v>
       </c>
       <c r="H48">
-        <v>151.51490000000001</v>
+        <v>132.5582</v>
       </c>
       <c r="I48" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000483890866178</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I48:I49" si="2">D48/H48</f>
+        <v>1.0000037719281039</v>
+      </c>
+      <c r="J48" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B49" s="5">
-        <v>2007</v>
+        <v>1995</v>
       </c>
       <c r="C49" s="3">
-        <v>0.46051274153983002</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="D49" s="1">
-        <v>7041.4958590400001</v>
-      </c>
-      <c r="E49" s="6">
-        <v>0</v>
-      </c>
+        <v>144.16820000000001</v>
+      </c>
+      <c r="E49" s="6"/>
       <c r="G49" s="8">
-        <v>0.4605127</v>
+        <v>0.35399700000000001</v>
       </c>
       <c r="H49">
-        <v>586.79129999999998</v>
+        <v>144.16829999999999</v>
       </c>
       <c r="I49" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000000441451672</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+        <f t="shared" si="2"/>
+        <v>0.99999930636624024</v>
+      </c>
+      <c r="J49" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B50" s="5">
         <v>1994</v>
       </c>
       <c r="C50" s="3">
-        <v>0.41525964898418</v>
+        <v>0.63240365126325004</v>
       </c>
       <c r="D50" s="1">
-        <v>495.27728671044002</v>
+        <v>1579.0311005271001</v>
       </c>
       <c r="E50" s="6">
-        <v>0.2575407356676</v>
+        <v>3.0019801980198002</v>
       </c>
       <c r="G50" s="8">
-        <v>0.41525590000000001</v>
+        <v>0.63240410000000002</v>
       </c>
       <c r="H50">
-        <v>41.272869999999998</v>
+        <v>131.58510000000001</v>
       </c>
       <c r="I50" s="9">
         <f t="shared" si="1"/>
-        <v>12.000068972921923</v>
+        <v>12.000075240487714</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B51" s="5">
-        <v>1992</v>
+        <v>1997</v>
       </c>
       <c r="C51" s="3">
-        <v>0.44984053655306999</v>
+        <v>0.34392591743202999</v>
       </c>
       <c r="D51" s="1">
-        <v>277.56252168863</v>
+        <v>3324.0256404453999</v>
       </c>
       <c r="E51" s="6">
-        <v>10.277243042483001</v>
+        <v>0</v>
       </c>
       <c r="G51" s="8">
-        <v>0.44984049999999998</v>
+        <v>0.34392590000000001</v>
       </c>
       <c r="H51">
-        <v>69.390630000000002</v>
+        <v>277.00209999999998</v>
       </c>
       <c r="I51" s="9">
         <f t="shared" si="1"/>
-        <v>4.0000000243351295</v>
+        <v>12.000001590043542</v>
       </c>
       <c r="J51" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B52" s="5">
-        <v>1996</v>
+        <v>1998</v>
       </c>
       <c r="C52" s="3">
-        <v>0.519222464439</v>
+        <v>0.33264852906081999</v>
       </c>
       <c r="D52" s="1">
-        <v>850.09963405927999</v>
+        <v>3389.7841033217001</v>
       </c>
       <c r="E52" s="6">
-        <v>0.68838765120324996</v>
+        <v>0</v>
       </c>
       <c r="G52" s="8">
-        <v>0.51922250000000003</v>
+        <v>0.33264850000000001</v>
       </c>
       <c r="H52">
-        <v>70.841639999999998</v>
+        <v>282.47070000000002</v>
       </c>
       <c r="I52" s="9">
         <f t="shared" si="1"/>
-        <v>11.999999351501179</v>
+        <v>12.000480415567703</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B53" s="5">
-        <v>1987</v>
+        <v>1997</v>
       </c>
       <c r="C53" s="3">
-        <v>0.33316897323624001</v>
+        <v>0.36942146402816001</v>
       </c>
       <c r="D53" s="1">
-        <v>746.71375954219002</v>
+        <v>1651.5335344744999</v>
       </c>
       <c r="E53" s="6">
-        <v>2.0320975514100002E-3</v>
+        <v>0</v>
       </c>
       <c r="G53" s="8">
-        <v>0.33316899999999999</v>
+        <v>0.36942150000000001</v>
       </c>
       <c r="H53">
-        <v>62.223660000000002</v>
+        <v>137.6223</v>
       </c>
       <c r="I53" s="9">
         <f t="shared" si="1"/>
-        <v>12.000479552989811</v>
+        <v>12.000479097315624</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B54" s="5">
-        <v>1996</v>
+        <v>2005</v>
       </c>
       <c r="C54" s="3">
-        <v>0.28664988638666</v>
+        <v>0.36281000000000002</v>
       </c>
       <c r="D54" s="1">
-        <v>1222.4380296459999</v>
+        <v>1711.1320000000001</v>
       </c>
       <c r="E54" s="6">
         <v>0</v>
       </c>
       <c r="G54" s="8">
-        <v>0.2866532</v>
+        <v>0.3627823</v>
       </c>
       <c r="H54">
-        <v>101.8704</v>
+        <v>142.59469999999999</v>
       </c>
       <c r="I54" s="9">
         <f t="shared" si="1"/>
-        <v>11.999933539536508</v>
+        <v>11.999969143313182</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B55" s="5">
-        <v>1998</v>
+        <v>1984</v>
       </c>
       <c r="C55" s="3">
-        <v>0.33123292700844997</v>
+        <v>0.48947361158580999</v>
       </c>
       <c r="D55" s="1">
-        <v>1216.1155325653999</v>
+        <v>298.99035500367</v>
       </c>
       <c r="E55" s="6">
-        <v>0</v>
+        <v>8.1377779613252006</v>
       </c>
       <c r="G55" s="8">
-        <v>0.33123659999999999</v>
+        <v>0.48947459999999998</v>
       </c>
       <c r="H55">
-        <v>101.3437</v>
+        <v>298.99160000000001</v>
       </c>
       <c r="I55" s="9">
         <f t="shared" si="1"/>
-        <v>11.99991250137305</v>
+        <v>0.99999583601569408</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B56" s="5">
-        <v>1985</v>
+        <v>1989</v>
       </c>
       <c r="C56" s="3">
-        <v>0.45634982338343999</v>
-      </c>
-      <c r="D56" s="2">
-        <v>40.368443077104999</v>
+        <v>0.54342483967208999</v>
+      </c>
+      <c r="D56" s="1">
+        <v>367.25653775262998</v>
       </c>
       <c r="E56" s="6">
-        <v>82.405237510693993</v>
+        <v>7.0811973975678004</v>
       </c>
       <c r="G56" s="8">
-        <v>0.45634980000000003</v>
+        <v>0.54342599999999996</v>
       </c>
       <c r="H56">
-        <v>403.68439999999998</v>
-      </c>
-      <c r="I56" s="10">
-        <f>D56/H56</f>
-        <v>0.10000000762255118</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+        <v>367.25450000000001</v>
+      </c>
+      <c r="I56" s="9">
+        <f t="shared" si="1"/>
+        <v>1.0000055486117392</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B57" s="5">
         <v>1994</v>
       </c>
       <c r="C57" s="3">
-        <v>0.44023988658683999</v>
+        <v>0.50441236709199</v>
       </c>
       <c r="D57" s="1">
-        <v>2355.4176102848</v>
+        <v>449.08490898819002</v>
       </c>
       <c r="E57" s="6">
-        <v>0</v>
+        <v>1.6730619539156999</v>
       </c>
       <c r="G57" s="8">
-        <v>0.44023990000000002</v>
+        <v>0.50441239999999998</v>
       </c>
       <c r="H57">
-        <v>196.27690000000001</v>
+        <v>37.422249999999998</v>
       </c>
       <c r="I57" s="9">
         <f t="shared" si="1"/>
-        <v>12.000483043520658</v>
+        <v>12.000478565243673</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B58" s="5">
-        <v>1988</v>
+        <v>2002</v>
       </c>
       <c r="C58" s="3">
-        <v>0.40746267421462001</v>
+        <v>0.32892948140056999</v>
       </c>
       <c r="D58" s="1">
-        <v>1497.0996781384999</v>
+        <v>1818.2521166762001</v>
       </c>
       <c r="E58" s="6">
         <v>0</v>
       </c>
       <c r="G58" s="8">
-        <v>0.40746270000000001</v>
+        <v>0.32892949999999999</v>
       </c>
       <c r="H58">
-        <v>124.7533</v>
+        <v>151.51490000000001</v>
       </c>
       <c r="I58" s="9">
         <f t="shared" si="1"/>
-        <v>12.000481575545496</v>
+        <v>12.000483890866178</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B59" s="5">
-        <v>1997</v>
+        <v>2007</v>
       </c>
       <c r="C59" s="3">
-        <v>0.45962207540877997</v>
+        <v>0.46051274153983002</v>
       </c>
       <c r="D59" s="1">
-        <v>24476.175033878</v>
+        <v>7041.4958590400001</v>
       </c>
       <c r="E59" s="6">
         <v>0</v>
       </c>
       <c r="G59" s="8">
-        <v>0.45962209999999998</v>
+        <v>0.4605127</v>
       </c>
       <c r="H59">
-        <v>169.9666</v>
+        <v>586.79129999999998</v>
       </c>
       <c r="I59" s="9">
         <f t="shared" si="1"/>
-        <v>144.00579310216241</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+        <v>12.000000441451672</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B60" s="5">
-        <v>1998</v>
+        <v>1994</v>
       </c>
       <c r="C60" s="3">
-        <v>0.31083240134617002</v>
+        <v>0.41525964898418</v>
       </c>
       <c r="D60" s="1">
-        <v>658.90832637027995</v>
+        <v>495.27728671044002</v>
       </c>
       <c r="E60" s="6">
-        <v>2.7530794588650001E-2</v>
+        <v>0.2575407356676</v>
       </c>
       <c r="G60" s="8">
-        <v>0.31083240000000001</v>
+        <v>0.41525590000000001</v>
       </c>
       <c r="H60">
-        <v>216.62739999999999</v>
+        <v>41.272869999999998</v>
       </c>
       <c r="I60" s="9">
         <f t="shared" si="1"/>
-        <v>3.0416665960551619</v>
+        <v>12.000068972921923</v>
       </c>
       <c r="J60" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B61" s="5">
-        <v>1999</v>
+        <v>1992</v>
       </c>
       <c r="C61" s="3">
-        <v>0.57609749096374996</v>
+        <v>0.44984053655306999</v>
       </c>
       <c r="D61" s="1">
-        <v>217.88215443623</v>
+        <v>277.56252168863</v>
       </c>
       <c r="E61" s="6">
-        <v>23.379730317528999</v>
+        <v>10.277243042483001</v>
       </c>
       <c r="G61" s="8">
-        <v>0.57609750000000004</v>
+        <v>0.44984049999999998</v>
       </c>
       <c r="H61">
-        <v>217.88220000000001</v>
+        <v>69.390630000000002</v>
       </c>
       <c r="I61" s="9">
         <f t="shared" si="1"/>
-        <v>0.99999979087887847</v>
+        <v>4.0000000243351295</v>
       </c>
       <c r="J61" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" s="5">
+        <v>1996</v>
+      </c>
+      <c r="C62" s="3">
+        <v>0.519222464439</v>
+      </c>
+      <c r="D62" s="1">
+        <v>850.09963405927999</v>
+      </c>
+      <c r="E62" s="6">
+        <v>0.68838765120324996</v>
+      </c>
+      <c r="G62" s="8">
+        <v>0.51922250000000003</v>
+      </c>
+      <c r="H62">
+        <v>70.841639999999998</v>
+      </c>
+      <c r="I62" s="9">
+        <f t="shared" si="1"/>
+        <v>11.999999351501179</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" s="5">
+        <v>1987</v>
+      </c>
+      <c r="C63" s="3">
+        <v>0.33316897323624001</v>
+      </c>
+      <c r="D63" s="1">
+        <v>746.71375954219002</v>
+      </c>
+      <c r="E63" s="6">
+        <v>2.0320975514100002E-3</v>
+      </c>
+      <c r="G63" s="8">
+        <v>0.33316899999999999</v>
+      </c>
+      <c r="H63">
+        <v>62.223660000000002</v>
+      </c>
+      <c r="I63" s="9">
+        <f>D63/H63</f>
+        <v>12.000479552989811</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" s="5">
+        <v>1990</v>
+      </c>
+      <c r="C64">
+        <v>0.3324857</v>
+      </c>
+      <c r="D64">
+        <v>63.231310000000001</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="G64">
+        <v>0.3324857</v>
+      </c>
+      <c r="H64">
+        <v>63.231310000000001</v>
+      </c>
+      <c r="I64" s="9">
+        <f>D64/H64</f>
+        <v>1</v>
+      </c>
+      <c r="J64" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A62" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B62" s="5">
-        <v>2002</v>
-      </c>
-      <c r="C62" s="3">
-        <v>0.29121610555256999</v>
-      </c>
-      <c r="D62" s="1">
-        <v>8949.9102047531997</v>
-      </c>
-      <c r="E62" s="6">
-        <v>0</v>
-      </c>
-      <c r="G62" s="8">
-        <v>0.29121609999999998</v>
-      </c>
-      <c r="H62">
-        <v>745.82539999999995</v>
-      </c>
-      <c r="I62" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000007246673551</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B63" s="5">
-        <v>2003</v>
-      </c>
-      <c r="C63" s="3">
-        <v>0.30866022853584002</v>
-      </c>
-      <c r="D63" s="1">
-        <v>8835.7881483052006</v>
-      </c>
-      <c r="E63" s="6">
-        <v>0</v>
-      </c>
-      <c r="G63" s="8">
-        <v>0.3086603</v>
-      </c>
-      <c r="H63">
-        <v>736.31600000000003</v>
-      </c>
-      <c r="I63" s="9">
-        <f t="shared" si="1"/>
-        <v>11.999994768964955</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A64" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B64" s="5">
-        <v>1999</v>
-      </c>
-      <c r="C64" s="3">
-        <v>0.42776691083605001</v>
-      </c>
-      <c r="D64" s="1">
-        <v>7010.5320259165001</v>
-      </c>
-      <c r="E64" s="6">
-        <v>0</v>
-      </c>
-      <c r="G64" s="8">
-        <v>0.42776690000000001</v>
-      </c>
-      <c r="H64">
-        <v>584.21050000000002</v>
-      </c>
-      <c r="I64" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000010314632311</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B65" s="5">
-        <v>2004</v>
+        <v>1996</v>
       </c>
       <c r="C65" s="3">
-        <v>0.35776169416289</v>
+        <v>0.28664988638666</v>
       </c>
       <c r="D65" s="1">
-        <v>2606.2084891575</v>
+        <v>1222.4380296459999</v>
       </c>
       <c r="E65" s="6">
         <v>0</v>
       </c>
       <c r="G65" s="8">
-        <v>0.35776170000000002</v>
+        <v>0.2866532</v>
       </c>
       <c r="H65">
-        <v>217.1754</v>
+        <v>101.8704</v>
       </c>
       <c r="I65" s="9">
         <f t="shared" si="1"/>
-        <v>12.000477444303085</v>
+        <v>11.999933539536508</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B66" s="5">
-        <v>1990</v>
+        <v>1998</v>
       </c>
       <c r="C66" s="3">
-        <v>0.45265648675885001</v>
+        <v>0.33123292700844997</v>
       </c>
       <c r="D66" s="1">
-        <v>2329.3012934230001</v>
+        <v>1216.1155325653999</v>
       </c>
       <c r="E66" s="6">
         <v>0</v>
       </c>
       <c r="G66" s="8">
-        <v>0.45265650000000002</v>
+        <v>0.33123659999999999</v>
       </c>
       <c r="H66">
-        <v>194.10069999999999</v>
+        <v>101.3437</v>
       </c>
       <c r="I66" s="9">
         <f t="shared" si="1"/>
-        <v>12.000478583657864</v>
+        <v>11.99991250137305</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B67" s="5">
-        <v>1992</v>
+        <v>1985</v>
       </c>
       <c r="C67" s="3">
-        <v>0.47857957837644</v>
-      </c>
-      <c r="D67" s="1">
-        <v>2803.8075951380001</v>
+        <v>0.45634982338343999</v>
+      </c>
+      <c r="D67" s="2">
+        <f xml:space="preserve"> 4843.881</f>
+        <v>4843.8810000000003</v>
       </c>
       <c r="E67" s="6">
-        <v>0</v>
+        <v>82.405237510693993</v>
       </c>
       <c r="G67" s="8">
-        <v>0.47857959999999999</v>
+        <v>0.45634980000000003</v>
       </c>
       <c r="H67">
-        <v>233.6413</v>
+        <v>403.68439999999998</v>
       </c>
       <c r="I67" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000479346493965</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+        <f>D67/H67</f>
+        <v>11.999178070789956</v>
+      </c>
+      <c r="J67" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B68" s="5">
         <v>1994</v>
       </c>
       <c r="C68" s="3">
-        <v>0.43470211763531003</v>
+        <v>0.44023988658683999</v>
       </c>
       <c r="D68" s="1">
-        <v>2947.8701410115</v>
+        <v>2355.4176102848</v>
       </c>
       <c r="E68" s="6">
         <v>0</v>
       </c>
       <c r="G68" s="8">
-        <v>0.43470209999999998</v>
+        <v>0.44023990000000002</v>
       </c>
       <c r="H68">
-        <v>245.64599999999999</v>
+        <v>196.27690000000001</v>
       </c>
       <c r="I68" s="9">
         <f t="shared" si="1"/>
-        <v>12.000480940098761</v>
+        <v>12.000483043520658</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B69" s="5">
-        <v>1996</v>
+        <v>1988</v>
       </c>
       <c r="C69" s="3">
-        <v>0.42904921347623998</v>
+        <v>0.40746267421462001</v>
       </c>
       <c r="D69" s="1">
-        <v>3200.9264543557001</v>
+        <v>1497.0996781384999</v>
       </c>
       <c r="E69" s="6">
         <v>0</v>
       </c>
       <c r="G69" s="8">
-        <v>0.42904920000000002</v>
+        <v>0.40746270000000001</v>
       </c>
       <c r="H69">
-        <v>266.73320000000001</v>
+        <v>124.7533</v>
       </c>
       <c r="I69" s="9">
         <f t="shared" si="1"/>
-        <v>12.000480084052903</v>
+        <v>12.000481575545496</v>
       </c>
       <c r="J69" s="4" t="s">
         <v>47</v>
@@ -2716,386 +2741,1055 @@
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B70" s="5">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="C70" s="3">
-        <v>0.41455794685635999</v>
+        <v>0.45962207540877997</v>
       </c>
       <c r="D70" s="1">
-        <v>3200.2666581018002</v>
+        <v>24476.175033878</v>
       </c>
       <c r="E70" s="6">
         <v>0</v>
       </c>
       <c r="G70" s="8">
-        <v>0.41455789999999998</v>
+        <v>0.45962209999999998</v>
       </c>
       <c r="H70">
-        <v>266.6782</v>
+        <v>169.9666</v>
       </c>
       <c r="I70" s="9">
-        <f t="shared" si="1"/>
-        <v>12.000480947080788</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+        <f>D70/H70</f>
+        <v>144.00579310216241</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B71" s="5">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="C71" s="3">
-        <v>0.43091587501703998</v>
+        <v>0.31083240134617002</v>
       </c>
       <c r="D71" s="1">
-        <v>3058.5604605226999</v>
+        <v>658.90832637027995</v>
       </c>
       <c r="E71" s="6">
-        <v>0</v>
+        <v>2.7530794588650001E-2</v>
       </c>
       <c r="G71" s="8">
-        <v>0.43091590000000002</v>
+        <v>0.31083240000000001</v>
       </c>
       <c r="H71">
-        <v>254.8698</v>
+        <v>216.62739999999999</v>
       </c>
       <c r="I71" s="9">
         <f t="shared" si="1"/>
-        <v>12.000482052101503</v>
+        <v>3.0416665960551619</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B72" s="5">
         <v>1999</v>
       </c>
       <c r="C72" s="3">
-        <v>0.43003754248201997</v>
+        <v>0.57609749096374996</v>
       </c>
       <c r="D72" s="1">
-        <v>8902.3533181845996</v>
+        <v>217.88215443623</v>
       </c>
       <c r="E72" s="6">
+        <v>23.379730317528999</v>
+      </c>
+      <c r="G72" s="8">
+        <v>0.57609750000000004</v>
+      </c>
+      <c r="H72">
+        <v>217.88220000000001</v>
+      </c>
+      <c r="I72" s="9">
+        <f t="shared" si="1"/>
+        <v>0.99999979087887847</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B73" s="5">
+        <v>2002</v>
+      </c>
+      <c r="C73" s="3">
+        <v>0.29121610555256999</v>
+      </c>
+      <c r="D73" s="1">
+        <v>8949.9102047531997</v>
+      </c>
+      <c r="E73" s="6">
         <v>0</v>
       </c>
-      <c r="G72" s="8">
-        <v>0.43003710000000001</v>
-      </c>
-      <c r="H72">
-        <v>61.821959999999997</v>
-      </c>
-      <c r="I72" s="9">
-        <f t="shared" si="1"/>
-        <v>143.99985568533577</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B73" s="5">
+      <c r="G73" s="8">
+        <v>0.29121609999999998</v>
+      </c>
+      <c r="H73">
+        <v>745.82539999999995</v>
+      </c>
+      <c r="I73" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000007246673551</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" s="5">
+        <v>2003</v>
+      </c>
+      <c r="C74" s="3">
+        <v>0.30866022853584002</v>
+      </c>
+      <c r="D74" s="1">
+        <v>8835.7881483052006</v>
+      </c>
+      <c r="E74" s="6">
+        <v>0</v>
+      </c>
+      <c r="G74" s="8">
+        <v>0.3086603</v>
+      </c>
+      <c r="H74">
+        <v>736.31600000000003</v>
+      </c>
+      <c r="I74" s="9">
+        <f t="shared" si="1"/>
+        <v>11.999994768964955</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="5">
+        <v>1999</v>
+      </c>
+      <c r="C75" s="3">
+        <v>0.42776691083605001</v>
+      </c>
+      <c r="D75" s="1">
+        <v>7010.5320259165001</v>
+      </c>
+      <c r="E75" s="6">
+        <v>0</v>
+      </c>
+      <c r="G75" s="8">
+        <v>0.42776690000000001</v>
+      </c>
+      <c r="H75">
+        <v>584.21050000000002</v>
+      </c>
+      <c r="I75" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000010314632311</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B76" s="5">
+        <v>2004</v>
+      </c>
+      <c r="C76" s="3">
+        <v>0.35776169416289</v>
+      </c>
+      <c r="D76" s="1">
+        <v>2606.2084891575</v>
+      </c>
+      <c r="E76" s="6">
+        <v>0</v>
+      </c>
+      <c r="G76" s="8">
+        <v>0.35776170000000002</v>
+      </c>
+      <c r="H76">
+        <v>217.1754</v>
+      </c>
+      <c r="I76" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000477444303085</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77" s="5">
+        <v>1990</v>
+      </c>
+      <c r="C77" s="3">
+        <v>0.45265648675885001</v>
+      </c>
+      <c r="D77" s="1">
+        <v>2329.3012934230001</v>
+      </c>
+      <c r="E77" s="6">
+        <v>0</v>
+      </c>
+      <c r="G77" s="8">
+        <v>0.45265650000000002</v>
+      </c>
+      <c r="H77">
+        <v>194.10069999999999</v>
+      </c>
+      <c r="I77" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000478583657864</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" s="5">
         <v>1992</v>
       </c>
-      <c r="C73" s="3">
-        <v>0.29708921417221001</v>
-      </c>
-      <c r="D73" s="1">
-        <v>211.77845247817999</v>
-      </c>
-      <c r="E73" s="6">
-        <v>2.9868533760381002</v>
-      </c>
-      <c r="G73" s="8">
-        <v>0.2970892</v>
-      </c>
-      <c r="H73">
-        <v>211.77850000000001</v>
-      </c>
-      <c r="I73" s="9">
-        <f t="shared" ref="I73:I82" si="2">D73/H73</f>
-        <v>0.99999977560602227</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A74" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B74" s="5">
-        <v>1993</v>
-      </c>
-      <c r="C74" s="3">
-        <v>0.28926983569553</v>
-      </c>
-      <c r="D74" s="1">
-        <v>212.96447526130001</v>
-      </c>
-      <c r="E74" s="6">
-        <v>1.3151858082275001</v>
-      </c>
-      <c r="G74" s="8">
-        <v>0.28926980000000002</v>
-      </c>
-      <c r="H74">
-        <v>212.96449999999999</v>
-      </c>
-      <c r="I74" s="9">
-        <f t="shared" si="2"/>
-        <v>0.99999988383650806</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B75" s="5">
-        <v>1996</v>
-      </c>
-      <c r="C75" s="3">
-        <v>0.35155947286084999</v>
-      </c>
-      <c r="D75" s="1">
-        <v>15.518902378802</v>
-      </c>
-      <c r="E75" s="6">
-        <v>98.712216061527002</v>
-      </c>
-      <c r="G75" s="8">
-        <v>0.35155950000000002</v>
-      </c>
-      <c r="H75">
-        <v>186.2268</v>
-      </c>
-      <c r="I75" s="10">
-        <f t="shared" si="2"/>
-        <v>8.3333346107015746E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A76" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B76" s="5">
-        <v>1998</v>
-      </c>
-      <c r="C76" s="3">
-        <v>0.44673173630141</v>
-      </c>
-      <c r="D76" s="1">
-        <v>95.072848027313</v>
-      </c>
-      <c r="E76" s="6">
-        <v>40.178586543573999</v>
-      </c>
-      <c r="G76" s="8">
-        <v>0.44673170000000001</v>
-      </c>
-      <c r="H76">
-        <v>95.072850000000003</v>
-      </c>
-      <c r="I76" s="9">
-        <f t="shared" si="2"/>
-        <v>0.99999997925078499</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A77" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B77" s="5">
-        <v>1992</v>
-      </c>
-      <c r="C77" s="3">
-        <v>0.35654558894558003</v>
-      </c>
-      <c r="D77" s="1">
-        <v>8.7898448694121001</v>
-      </c>
-      <c r="E77" s="6">
-        <v>99.773480431226005</v>
-      </c>
-      <c r="G77" s="8">
-        <v>0.35654400000000003</v>
-      </c>
-      <c r="H77">
-        <v>73.24821</v>
-      </c>
-      <c r="I77" s="10">
-        <f t="shared" si="2"/>
-        <v>0.12000081461938933</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A78" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B78" s="5">
-        <v>1998</v>
-      </c>
       <c r="C78" s="3">
-        <v>0.3544220745503</v>
+        <v>0.47857957837644</v>
       </c>
       <c r="D78" s="1">
-        <v>11.033454573153</v>
+        <v>2803.8075951380001</v>
       </c>
       <c r="E78" s="6">
-        <v>99.466938516203001</v>
+        <v>0</v>
       </c>
       <c r="G78" s="8">
-        <v>0.35442259999999998</v>
+        <v>0.47857959999999999</v>
       </c>
       <c r="H78">
-        <v>91.945509999999999</v>
-      </c>
-      <c r="I78" s="10">
-        <f t="shared" si="2"/>
-        <v>0.11999992792636638</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+        <v>233.6413</v>
+      </c>
+      <c r="I78" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000479346493965</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B79" s="5">
-        <v>1998</v>
+        <v>1994</v>
       </c>
       <c r="C79" s="3">
-        <v>0.34997786461265001</v>
+        <v>0.43470211763531003</v>
       </c>
       <c r="D79" s="1">
-        <v>2064.8187468602</v>
+        <v>2947.8701410115</v>
       </c>
       <c r="E79" s="6">
         <v>0</v>
       </c>
       <c r="G79" s="8">
-        <v>0.34997790000000001</v>
+        <v>0.43470209999999998</v>
       </c>
       <c r="H79">
-        <v>172.06129999999999</v>
+        <v>245.64599999999999</v>
       </c>
       <c r="I79" s="9">
-        <f t="shared" si="2"/>
-        <v>12.000483239753507</v>
+        <f t="shared" si="1"/>
+        <v>12.000480940098761</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B80" s="5">
-        <v>2008</v>
+        <v>1996</v>
       </c>
       <c r="C80" s="3">
-        <v>0.63008997319922</v>
+        <v>0.42904921347623998</v>
       </c>
       <c r="D80" s="1">
-        <v>4080.4488455433002</v>
+        <v>3200.9264543557001</v>
       </c>
       <c r="E80" s="6">
         <v>0</v>
       </c>
       <c r="G80" s="8">
+        <v>0.42904920000000002</v>
+      </c>
+      <c r="H80">
+        <v>266.73320000000001</v>
+      </c>
+      <c r="I80" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000480084052903</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" s="5">
+        <v>1998</v>
+      </c>
+      <c r="C81" s="3">
+        <v>0.41455794685635999</v>
+      </c>
+      <c r="D81" s="1">
+        <v>3200.2666581018002</v>
+      </c>
+      <c r="E81" s="6">
+        <v>0</v>
+      </c>
+      <c r="G81" s="8">
+        <v>0.41455789999999998</v>
+      </c>
+      <c r="H81">
+        <v>266.6782</v>
+      </c>
+      <c r="I81" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000480947080788</v>
+      </c>
+      <c r="J81" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="5">
+        <v>1999</v>
+      </c>
+      <c r="C82" s="3">
+        <v>0.43091587501703998</v>
+      </c>
+      <c r="D82" s="1">
+        <v>3058.5604605226999</v>
+      </c>
+      <c r="E82" s="6">
+        <v>0</v>
+      </c>
+      <c r="G82" s="8">
+        <v>0.43091590000000002</v>
+      </c>
+      <c r="H82">
+        <v>254.8698</v>
+      </c>
+      <c r="I82" s="9">
+        <f t="shared" si="1"/>
+        <v>12.000482052101503</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" s="5">
+        <v>1999</v>
+      </c>
+      <c r="C83" s="3">
+        <v>0.43003754248201997</v>
+      </c>
+      <c r="D83" s="1">
+        <v>8902.3533181845996</v>
+      </c>
+      <c r="E83" s="6">
+        <v>0</v>
+      </c>
+      <c r="G83" s="8">
+        <v>0.43003710000000001</v>
+      </c>
+      <c r="H83">
+        <v>61.821959999999997</v>
+      </c>
+      <c r="I83" s="9">
+        <f t="shared" si="1"/>
+        <v>143.99985568533577</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" s="5">
+        <v>1992</v>
+      </c>
+      <c r="C84" s="3">
+        <v>0.29708921417221001</v>
+      </c>
+      <c r="D84" s="1">
+        <v>211.77845247817999</v>
+      </c>
+      <c r="E84" s="6">
+        <v>2.9868533760381002</v>
+      </c>
+      <c r="G84" s="8">
+        <v>0.2970892</v>
+      </c>
+      <c r="H84">
+        <v>211.77850000000001</v>
+      </c>
+      <c r="I84" s="9">
+        <f t="shared" ref="I84:I104" si="3">D84/H84</f>
+        <v>0.99999977560602227</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" s="5">
+        <v>1993</v>
+      </c>
+      <c r="C85" s="3">
+        <v>0.28926983569553</v>
+      </c>
+      <c r="D85" s="1">
+        <v>212.96447526130001</v>
+      </c>
+      <c r="E85" s="6">
+        <v>1.3151858082275001</v>
+      </c>
+      <c r="G85" s="8">
+        <v>0.28926980000000002</v>
+      </c>
+      <c r="H85">
+        <v>212.96449999999999</v>
+      </c>
+      <c r="I85" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999988383650806</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" s="5">
+        <v>1996</v>
+      </c>
+      <c r="C86" s="3">
+        <v>0.35155947286084999</v>
+      </c>
+      <c r="D86" s="1">
+        <v>186.2268</v>
+      </c>
+      <c r="E86" s="6">
+        <v>5.3659999999999997</v>
+      </c>
+      <c r="G86" s="8">
+        <v>0.35155950000000002</v>
+      </c>
+      <c r="H86">
+        <v>186.2268</v>
+      </c>
+      <c r="I86" s="9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="5">
+        <v>1998</v>
+      </c>
+      <c r="C87" s="3">
+        <v>0.44673173630141</v>
+      </c>
+      <c r="D87" s="1">
+        <v>95.072848027313</v>
+      </c>
+      <c r="E87" s="6">
+        <v>40.178586543573999</v>
+      </c>
+      <c r="G87" s="8">
+        <v>0.44673170000000001</v>
+      </c>
+      <c r="H87">
+        <v>95.072850000000003</v>
+      </c>
+      <c r="I87" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999997925078499</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B88" s="4">
+        <v>1989</v>
+      </c>
+      <c r="C88">
+        <v>0.45294778000000002</v>
+      </c>
+      <c r="D88">
+        <v>361.05986000000001</v>
+      </c>
+      <c r="E88">
+        <v>7.3925441000000003</v>
+      </c>
+      <c r="G88">
+        <v>0.45295049999999998</v>
+      </c>
+      <c r="H88">
+        <v>361.06220000000002</v>
+      </c>
+      <c r="I88" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999351912219003</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A89" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B89" s="4">
+        <v>1992</v>
+      </c>
+      <c r="C89">
+        <v>0.42506241</v>
+      </c>
+      <c r="D89">
+        <v>340.24853999999999</v>
+      </c>
+      <c r="E89">
+        <v>4.8362610000000004</v>
+      </c>
+      <c r="G89">
+        <v>0.42506240000000001</v>
+      </c>
+      <c r="H89">
+        <v>340.24810000000002</v>
+      </c>
+      <c r="I89" s="9">
+        <f t="shared" si="3"/>
+        <v>1.0000012931740103</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B90" s="4">
+        <v>1995</v>
+      </c>
+      <c r="C90">
+        <v>0.47824907999999999</v>
+      </c>
+      <c r="D90">
+        <v>271.35557</v>
+      </c>
+      <c r="E90">
+        <v>10.413252</v>
+      </c>
+      <c r="G90">
+        <v>0.47824939999999999</v>
+      </c>
+      <c r="H90">
+        <v>271.35559999999998</v>
+      </c>
+      <c r="I90" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999988944396212</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91" s="4">
+        <v>1998</v>
+      </c>
+      <c r="C91">
+        <v>0.49803879000000001</v>
+      </c>
+      <c r="D91">
+        <v>278.14319</v>
+      </c>
+      <c r="E91">
+        <v>12.790533999999999</v>
+      </c>
+      <c r="G91">
+        <v>0.49803829999999999</v>
+      </c>
+      <c r="H91">
+        <v>278.1438</v>
+      </c>
+      <c r="I91" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999780688981743</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B92" s="4">
+        <v>1999</v>
+      </c>
+      <c r="C92">
+        <v>0.48324476</v>
+      </c>
+      <c r="D92">
+        <v>258.46044000000001</v>
+      </c>
+      <c r="E92">
+        <v>12.015749</v>
+      </c>
+      <c r="G92">
+        <v>0.48324400000000001</v>
+      </c>
+      <c r="H92">
+        <v>258.45890000000003</v>
+      </c>
+      <c r="I92" s="9">
+        <f t="shared" si="3"/>
+        <v>1.0000059583941585</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A93" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B93" s="4">
+        <v>2001</v>
+      </c>
+      <c r="C93">
+        <v>0.48223701000000002</v>
+      </c>
+      <c r="D93">
+        <v>269.55572000000001</v>
+      </c>
+      <c r="E93">
+        <v>10.963222</v>
+      </c>
+      <c r="G93">
+        <v>0.48224220000000001</v>
+      </c>
+      <c r="H93">
+        <v>269.55860000000001</v>
+      </c>
+      <c r="I93" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99998931586675399</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B94" s="4">
+        <v>2002</v>
+      </c>
+      <c r="C94">
+        <v>0.50557593000000001</v>
+      </c>
+      <c r="D94">
+        <v>218.63381999999999</v>
+      </c>
+      <c r="E94">
+        <v>18.228956</v>
+      </c>
+      <c r="G94">
+        <v>0.50557810000000003</v>
+      </c>
+      <c r="H94">
+        <v>218.63589999999999</v>
+      </c>
+      <c r="I94" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999048646631228</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B95" s="4">
+        <v>2003</v>
+      </c>
+      <c r="C95">
+        <v>0.50372634999999999</v>
+      </c>
+      <c r="D95">
+        <v>181.67498000000001</v>
+      </c>
+      <c r="E95">
+        <v>22.714452000000001</v>
+      </c>
+      <c r="G95">
+        <v>0.50372779999999995</v>
+      </c>
+      <c r="H95">
+        <v>181.6764</v>
+      </c>
+      <c r="I95" s="9">
+        <f t="shared" si="3"/>
+        <v>0.9999921839050091</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A96" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B96" s="4">
+        <v>2004</v>
+      </c>
+      <c r="C96">
+        <v>0.49819235000000001</v>
+      </c>
+      <c r="D96">
+        <v>203.66030000000001</v>
+      </c>
+      <c r="E96">
+        <v>19.757425999999999</v>
+      </c>
+      <c r="G96">
+        <v>0.49819160000000001</v>
+      </c>
+      <c r="H96">
+        <v>203.65969999999999</v>
+      </c>
+      <c r="I96" s="9">
+        <f t="shared" si="3"/>
+        <v>1.0000029460909547</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B97" s="4">
+        <v>2005</v>
+      </c>
+      <c r="C97">
+        <v>0.52364754000000002</v>
+      </c>
+      <c r="D97">
+        <v>251.35269</v>
+      </c>
+      <c r="E97">
+        <v>18.855108000000001</v>
+      </c>
+      <c r="G97">
+        <v>0.5236497</v>
+      </c>
+      <c r="H97">
+        <v>251.35400000000001</v>
+      </c>
+      <c r="I97" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999478822696275</v>
+      </c>
+      <c r="J97" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A98" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B98" s="4">
+        <v>2006</v>
+      </c>
+      <c r="C98">
+        <v>0.46940981999999998</v>
+      </c>
+      <c r="D98">
+        <v>314.80327</v>
+      </c>
+      <c r="E98">
+        <v>10.224276</v>
+      </c>
+      <c r="G98">
+        <v>0.46941310000000003</v>
+      </c>
+      <c r="H98">
+        <v>314.80590000000001</v>
+      </c>
+      <c r="I98" s="9">
+        <f t="shared" si="3"/>
+        <v>0.99999164564577725</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A99" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B99" s="5">
+        <v>1992</v>
+      </c>
+      <c r="C99" s="3">
+        <v>0.35654558894558003</v>
+      </c>
+      <c r="D99" s="1">
+        <v>8.7898448694121001</v>
+      </c>
+      <c r="E99" s="6">
+        <v>99.773480431226005</v>
+      </c>
+      <c r="G99" s="8">
+        <v>0.35654400000000003</v>
+      </c>
+      <c r="H99">
+        <v>73.24821</v>
+      </c>
+      <c r="I99" s="10">
+        <f t="shared" si="3"/>
+        <v>0.12000081461938933</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A100" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B100" s="5">
+        <v>1998</v>
+      </c>
+      <c r="C100" s="3">
+        <v>0.3544220745503</v>
+      </c>
+      <c r="D100" s="1">
+        <v>11.033454573153</v>
+      </c>
+      <c r="E100" s="6">
+        <v>99.466938516203001</v>
+      </c>
+      <c r="G100" s="8">
+        <v>0.35442259999999998</v>
+      </c>
+      <c r="H100">
+        <v>91.945509999999999</v>
+      </c>
+      <c r="I100" s="10">
+        <f t="shared" si="3"/>
+        <v>0.11999992792636638</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B101" s="5">
+        <v>1998</v>
+      </c>
+      <c r="C101" s="3">
+        <v>0.34997786461265001</v>
+      </c>
+      <c r="D101" s="1">
+        <v>2064.8187468602</v>
+      </c>
+      <c r="E101" s="6">
+        <v>0</v>
+      </c>
+      <c r="G101" s="8">
+        <v>0.34997790000000001</v>
+      </c>
+      <c r="H101">
+        <v>172.06129999999999</v>
+      </c>
+      <c r="I101" s="9">
+        <f t="shared" si="3"/>
+        <v>12.000483239753507</v>
+      </c>
+      <c r="J101" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B102" s="5">
+        <v>2008</v>
+      </c>
+      <c r="C102" s="3">
+        <v>0.63008997319922</v>
+      </c>
+      <c r="D102" s="1">
+        <v>4080.4488455433002</v>
+      </c>
+      <c r="E102" s="6">
+        <v>0</v>
+      </c>
+      <c r="G102" s="8">
         <v>0.63009099999999996</v>
       </c>
-      <c r="H80">
+      <c r="H102">
         <v>340.03789999999998</v>
       </c>
-      <c r="I80" s="9">
-        <f t="shared" si="2"/>
+      <c r="I102" s="9">
+        <f t="shared" si="3"/>
         <v>11.999982488844038</v>
       </c>
-      <c r="J80" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
+      <c r="J102" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A103" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B103" s="5">
         <v>1991</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C103" s="3">
         <v>0.60506191411084997</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D103" s="1">
         <f>1120873.8532464/12</f>
         <v>93406.154437199992</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E103" s="6">
         <v>5.33535189434E-3</v>
       </c>
-      <c r="G81" s="8">
+      <c r="G103" s="8">
         <v>0.60506190000000004</v>
       </c>
-      <c r="H81">
+      <c r="H103">
         <v>93.402420000000006</v>
       </c>
-      <c r="I81" s="9">
-        <f t="shared" si="2"/>
+      <c r="I103" s="9">
+        <f t="shared" si="3"/>
         <v>1000.0399822317236</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="J103" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A82" s="4" t="s">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B104" s="5">
         <v>2002</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C104" s="3">
         <v>0.42061926085369999</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D104" s="1">
         <f>989015.74930161/12</f>
         <v>82417.979108467509</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E104" s="6">
         <v>0</v>
       </c>
-      <c r="G82" s="8">
+      <c r="G104" s="8">
         <v>0.42061759999999998</v>
       </c>
-      <c r="H82">
+      <c r="H104">
         <v>82.417829999999995</v>
       </c>
-      <c r="I82" s="9">
-        <f t="shared" si="2"/>
+      <c r="I104" s="9">
+        <f t="shared" si="3"/>
         <v>1000.0018091773044</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="J104" s="4" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J82" xr:uid="{D6655631-472D-44CB-AAED-119A64067122}"/>
+  <autoFilter ref="A1:J104" xr:uid="{D6655631-472D-44CB-AAED-119A64067122}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="0.12"/>
+        <filter val="100"/>
+        <filter val="1000"/>
+        <filter val="144"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates on means check & conversion factors
</commit_message>
<xml_diff>
--- a/Check means on HIST data.xlsx
+++ b/Check means on HIST data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\02.personal\wb463998\Historical data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15EE9667-A6CC-484D-AD76-FAF11EE19FCE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1355EA6-769C-43D4-A456-C77660D131A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="62">
   <si>
     <t>countrycode</t>
   </si>
@@ -208,17 +208,30 @@
   </si>
   <si>
     <t>LKA</t>
+  </si>
+  <si>
+    <t>el ccf debe ser 275,000,000,000 ( está como 275,000,000 en pcn load cpi, clear)</t>
+  </si>
+  <si>
+    <t>el ccf debe ser 1000 (está como 1 en pcn load cpi, clear)</t>
+  </si>
+  <si>
+    <t>STILL A MISTERY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="6">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="_(* #,##0.00000000_);_(* \(#,##0.00000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0.00000000000_);_(* \(#,##0.00000000000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -236,6 +249,16 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -283,10 +306,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -327,8 +351,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -642,10 +673,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J104"/>
+  <dimension ref="A1:S106"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L104" sqref="L104"/>
+      <selection activeCell="L107" sqref="L107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -659,9 +690,12 @@
     <col min="7" max="8" width="9.90625" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
     <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="12" max="12" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -689,8 +723,9 @@
       <c r="J1" s="17" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="20"/>
+    </row>
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -721,7 +756,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -751,7 +786,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -781,7 +816,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -812,7 +847,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -843,7 +878,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -874,7 +909,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -904,7 +939,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
@@ -934,7 +969,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
@@ -964,7 +999,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
@@ -994,7 +1029,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1024,7 +1059,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -1054,7 +1089,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -1084,7 +1119,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -1114,8 +1149,11 @@
       <c r="J15" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L15" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -1145,8 +1183,11 @@
       <c r="J16" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L16" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
@@ -1176,8 +1217,11 @@
       <c r="J17" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L17" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -1207,8 +1251,11 @@
       <c r="J18" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L18" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -1238,8 +1285,11 @@
       <c r="J19" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L19" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -1265,8 +1315,11 @@
         <f t="shared" ref="I20:I83" si="1">D20/H20</f>
         <v>999.99995716577189</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L20" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -1292,8 +1345,11 @@
         <f t="shared" si="1"/>
         <v>999.99990366565441</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L21" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
@@ -1319,8 +1375,11 @@
         <f t="shared" si="1"/>
         <v>1000.0000688139837</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+      <c r="L22" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -1350,7 +1409,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1439,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>55</v>
       </c>
@@ -1410,7 +1469,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>56</v>
       </c>
@@ -1440,7 +1499,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>56</v>
       </c>
@@ -1470,7 +1529,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>56</v>
       </c>
@@ -1500,7 +1559,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
@@ -1530,7 +1589,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>8</v>
       </c>
@@ -1560,7 +1619,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>9</v>
       </c>
@@ -1590,7 +1649,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>10</v>
       </c>
@@ -1620,6 +1679,9 @@
       <c r="J32" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="L32" s="25" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
@@ -2739,7 +2801,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>29</v>
       </c>
@@ -2750,7 +2812,8 @@
         <v>0.45962207540877997</v>
       </c>
       <c r="D70" s="1">
-        <v>24476.175033878</v>
+        <f xml:space="preserve"> 2039.682</f>
+        <v>2039.682</v>
       </c>
       <c r="E70" s="6">
         <v>0</v>
@@ -2763,7 +2826,10 @@
       </c>
       <c r="I70" s="9">
         <f>D70/H70</f>
-        <v>144.00579310216241</v>
+        <v>12.000487154535067</v>
+      </c>
+      <c r="J70" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -3126,7 +3192,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>36</v>
       </c>
@@ -3137,7 +3203,8 @@
         <v>0.43003754248201997</v>
       </c>
       <c r="D83" s="1">
-        <v>8902.3533181845996</v>
+        <f>8902.3533181846/12</f>
+        <v>741.8627765153833</v>
       </c>
       <c r="E83" s="6">
         <v>0</v>
@@ -3150,7 +3217,10 @@
       </c>
       <c r="I83" s="9">
         <f t="shared" si="1"/>
-        <v>143.99985568533577</v>
+        <v>11.99998797377798</v>
+      </c>
+      <c r="J83" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -3543,7 +3613,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>57</v>
       </c>
@@ -3573,7 +3643,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>57</v>
       </c>
@@ -3603,7 +3673,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>39</v>
       </c>
@@ -3614,7 +3684,7 @@
         <v>0.35654558894558003</v>
       </c>
       <c r="D99" s="1">
-        <v>8.7898448694121001</v>
+        <v>73.248720000000006</v>
       </c>
       <c r="E99" s="6">
         <v>99.773480431226005</v>
@@ -3625,12 +3695,15 @@
       <c r="H99">
         <v>73.24821</v>
       </c>
-      <c r="I99" s="10">
+      <c r="I99" s="9">
         <f t="shared" si="3"/>
-        <v>0.12000081461938933</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.0000069626274828</v>
+      </c>
+      <c r="J99" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>39</v>
       </c>
@@ -3641,7 +3714,7 @@
         <v>0.3544220745503</v>
       </c>
       <c r="D100" s="1">
-        <v>11.033454573153</v>
+        <v>91.945449999999994</v>
       </c>
       <c r="E100" s="6">
         <v>99.466938516203001</v>
@@ -3652,12 +3725,15 @@
       <c r="H100">
         <v>91.945509999999999</v>
       </c>
-      <c r="I100" s="10">
+      <c r="I100" s="9">
         <f t="shared" si="3"/>
-        <v>0.11999992792636638</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+        <v>0.99999934743958674</v>
+      </c>
+      <c r="J100" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>40</v>
       </c>
@@ -3687,7 +3763,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:19" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>41</v>
       </c>
@@ -3717,7 +3793,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>42</v>
       </c>
@@ -3747,8 +3823,13 @@
       <c r="J103" s="4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="L103" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="R103" s="23"/>
+      <c r="S103" s="23"/>
+    </row>
+    <row r="104" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>42</v>
       </c>
@@ -3778,15 +3859,20 @@
       <c r="J104" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="L104" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="R104" s="24"/>
+    </row>
+    <row r="106" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="L106" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J104" xr:uid="{D6655631-472D-44CB-AAED-119A64067122}">
     <filterColumn colId="8">
       <filters>
-        <filter val="0.12"/>
         <filter val="100"/>
         <filter val="1000"/>
-        <filter val="144"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>